<commit_message>
feat: update Excel files with new data
Modified the binary files `XLMathCopy.xlsx` and `XLMathOriginal.xlsx`. The exact changes are not detailed in the diff output, but there are differences between the original and the copy, indicating updates or modifications to the data within these Excel files.
</commit_message>
<xml_diff>
--- a/SciCalcDemo/assets/XLMathCopy.xlsx
+++ b/SciCalcDemo/assets/XLMathCopy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A\source\repos\SciCalc\SciCalcDemo\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27F3D38-BCAB-4411-9EB1-351E74B5722E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCE1ACE-529B-4081-8F7C-32846CD1D0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{163E41E0-9AD6-4D75-8144-1BB501121731}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Num1</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
 </sst>
 </file>
@@ -461,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9E972E-3B3D-4BA3-93D4-345B3EF802EB}">
-  <dimension ref="A1:XFB9"/>
+  <dimension ref="A1:XFB11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +512,7 @@
         <v>17.773399999999999</v>
       </c>
       <c r="D2" s="1">
-        <v>6.4333999999999998</v>
+        <v>0.1134</v>
       </c>
       <c r="E2" s="1">
         <v>68.626277999999999</v>
@@ -524,13 +521,13 @@
         <v>2.134638448</v>
       </c>
       <c r="G2" s="1">
-        <v>41.980200000000004</v>
+        <v>104.286478</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="XFB2">
-        <v>41.980200000000004</v>
+        <v>104.286478</v>
       </c>
     </row>
     <row r="3" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
@@ -553,13 +550,13 @@
         <v>12.34</v>
       </c>
       <c r="G3" s="1">
-        <v>0.38019999999999998</v>
+        <v>0.381434</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="XFB3">
-        <v>0.38019999999999998</v>
+        <v>0.381434</v>
       </c>
     </row>
     <row r="4" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
@@ -582,13 +579,13 @@
         <v>0.112181818</v>
       </c>
       <c r="G4" s="1">
-        <v>1.4702</v>
+        <v>1.6059399999999999</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="XFB4">
-        <v>1.4702</v>
+        <v>1.6059399999999999</v>
       </c>
     </row>
     <row r="5" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
@@ -611,13 +608,13 @@
         <v>0.112181818</v>
       </c>
       <c r="G5" s="1">
-        <v>1.4702</v>
+        <v>1.6059399999999999</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="XFB5">
-        <v>1.4702</v>
+        <v>1.6059399999999999</v>
       </c>
     </row>
     <row r="6" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
@@ -640,13 +637,13 @@
         <v>0.1234</v>
       </c>
       <c r="G6" s="1">
-        <v>0.13702</v>
+        <v>0.13825399999999999</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="XFB6">
-        <v>0.13702</v>
+        <v>0.13825399999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
@@ -669,13 +666,13 @@
         <v>10.1234</v>
       </c>
       <c r="G7" s="1">
-        <v>3.1370200000000001</v>
+        <v>3.238254</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="XFB7">
-        <v>3.1370200000000001</v>
+        <v>3.238254</v>
       </c>
     </row>
     <row r="8" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
@@ -698,7 +695,7 @@
         <v>2.1346425830000002</v>
       </c>
       <c r="G8" s="1">
-        <v>41.980270339999997</v>
+        <v>110.60668130000001</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>8</v>
@@ -724,9 +721,61 @@
         <v>21.358628469999999</v>
       </c>
       <c r="G9" s="1">
-        <v>368.98027029999997</v>
+        <v>1055.636681</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>405.12345679999999</v>
+      </c>
+      <c r="B10" s="1">
+        <v>102.1234568</v>
+      </c>
+      <c r="C10" s="1">
+        <v>507.24691360000003</v>
+      </c>
+      <c r="D10" s="1">
+        <v>303</v>
+      </c>
+      <c r="E10" s="1">
+        <v>41372.607830000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3.9669970989999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>42690.10166</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8 16382:16382" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.99234500000000003</v>
+      </c>
+      <c r="C11" s="1">
+        <v>123456790</v>
+      </c>
+      <c r="D11" s="1">
+        <v>123456788</v>
+      </c>
+      <c r="E11" s="1">
+        <v>122511727.3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>124409141</v>
+      </c>
+      <c r="G11" s="1">
+        <v>492882095.30000001</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>